<commit_message>
test case with steps
</commit_message>
<xml_diff>
--- a/Test case.xlsx
+++ b/Test case.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuri\Desktop\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuri\Desktop\testing\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>requirement</t>
   </si>
@@ -60,6 +60,10 @@
   </si>
   <si>
     <t>go to the site</t>
+  </si>
+  <si>
+    <t>1. fill all fields
+2. click the button OK</t>
   </si>
 </sst>
 </file>
@@ -465,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -540,7 +544,9 @@
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "test case 2"
This reverts commit e8047ac6addd630687279a2ca1c632ab66d84280.
</commit_message>
<xml_diff>
--- a/Test case.xlsx
+++ b/Test case.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>requirement</t>
   </si>
@@ -63,10 +63,6 @@
   </si>
   <si>
     <t>1. fill all fields
-2. click the button OK</t>
-  </si>
-  <si>
-    <t>1. don't fill all fields
 2. click the button OK</t>
   </si>
 </sst>
@@ -474,7 +470,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -561,9 +557,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>